<commit_message>
Full update on the files
</commit_message>
<xml_diff>
--- a/man_tests_T1A2.xlsx
+++ b/man_tests_T1A2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shelbyd/CODING/Projects/Ruby/T1A2_Terminal_App/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shelbyd/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F4A5ED-AD44-2B41-8F7D-279A54694525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4512CA9B-D4AB-574C-8028-1205F528B31E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35420" yWindow="-3140" windowWidth="25540" windowHeight="16680" xr2:uid="{E4B1E5C7-DAD6-3D4D-9E2A-0CE9718F5B2E}"/>
+    <workbookView xWindow="34780" yWindow="-2900" windowWidth="24460" windowHeight="17320" xr2:uid="{E4B1E5C7-DAD6-3D4D-9E2A-0CE9718F5B2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Feature being tested</t>
   </si>
@@ -68,13 +68,118 @@
     <t>Test Case</t>
   </si>
   <si>
-    <t>Player Name</t>
-  </si>
-  <si>
     <t>Check results on entering a valid username</t>
   </si>
   <si>
     <t>Check results on entering a invalid username</t>
+  </si>
+  <si>
+    <t>Weapon Choice</t>
+  </si>
+  <si>
+    <t>Check results on entering a invalid weapon choice</t>
+  </si>
+  <si>
+    <t>Computer Player</t>
+  </si>
+  <si>
+    <t>Score Total</t>
+  </si>
+  <si>
+    <t>Check Score Total After Each Round</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check if a tie is reached the game loops again </t>
+  </si>
+  <si>
+    <t>Check that Once a player reachs score 5 there is a winner</t>
+  </si>
+  <si>
+    <t>Check results on entering a valid weapon choice</t>
+  </si>
+  <si>
+    <t>Check if a weapon is randomized for the computer</t>
+  </si>
+  <si>
+    <t>Play Again</t>
+  </si>
+  <si>
+    <t>Check results on entering an invalid key input for play again</t>
+  </si>
+  <si>
+    <t>Check results on entering an valid key input for play again</t>
+  </si>
+  <si>
+    <t>Check that the play again method restarts the game at the welcome message.</t>
+  </si>
+  <si>
+    <t>Rules_engine</t>
+  </si>
+  <si>
+    <t>Check when a round draws</t>
+  </si>
+  <si>
+    <t>Main Game- Player name</t>
+  </si>
+  <si>
+    <t>Game Round Class</t>
+  </si>
+  <si>
+    <t>As Expected</t>
+  </si>
+  <si>
+    <t>Passed!</t>
+  </si>
+  <si>
+    <t>S El-rassi</t>
+  </si>
+  <si>
+    <t>Check when a it’s a win for the computer</t>
+  </si>
+  <si>
+    <t>Check when a it’s a win for the Player</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if player_move == :scissors and computer_move == :paper 
+			:first                              so the first move will be the winning move </t>
+  </si>
+  <si>
+    <t>computer_move == :scissors and player_move == :paper 
+			:firs t              so the first move will be the winning move</t>
+  </si>
+  <si>
+    <t>assert_include(Weapons::ENTRY, 'r', message = nil)</t>
+  </si>
+  <si>
+    <t>Check that the Hash called ENTRY, included the string key</t>
+  </si>
+  <si>
+    <t>if player_move == computer_move the result would be a draw</t>
+  </si>
+  <si>
+    <t>Yes it does include</t>
+  </si>
+  <si>
+    <t>Checked that the called the Constant Hash Computer Choices index would equal the text I gave it</t>
+  </si>
+  <si>
+    <t>choice = Weapons::COMPUTER_CHOICES[0]
+        assert_equal(:ROCK, choice)</t>
+  </si>
+  <si>
+    <t>outcome = RulesEngine::round_draw(:rock, :rock)
+        assert_equal(:draw, outcome) round_draw(:scissors :scissors)</t>
+  </si>
+  <si>
+    <t>outcome = RulesEngine::player_win(:scissors, :paper)
+        assert_equal(:first, outcome)</t>
+  </si>
+  <si>
+    <t>outcome = RulesEngine::computer_win(:scissors, :paper)
+        assert_equal(:first, outcome)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes it does equal </t>
   </si>
 </sst>
 </file>
@@ -103,12 +208,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -123,10 +240,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,95 +579,407 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB52CDC-51B2-5744-8C62-74681603DE00}">
-  <dimension ref="A2:K8"/>
+  <dimension ref="A2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" style="2" customWidth="1"/>
-    <col min="4" max="9" width="22.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="22.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18" style="1" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" customWidth="1"/>
     <col min="11" max="11" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="2">
+        <v>43943</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>3</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="C12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="B13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="B14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
         <v>6</v>
       </c>
+      <c r="B15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>7</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>8</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>9</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>10</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>11</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bulk push to update github
</commit_message>
<xml_diff>
--- a/man_tests_T1A2.xlsx
+++ b/man_tests_T1A2.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shelbyd/CODING/Projects/Ruby/CA_Terminal_App_RPSLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED77C817-E7A3-ED44-8DCC-BC69D8A33683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8470F2-7517-3349-9117-424DD0F64F7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3940" windowWidth="30600" windowHeight="18120" xr2:uid="{E4B1E5C7-DAD6-3D4D-9E2A-0CE9718F5B2E}"/>
+    <workbookView xWindow="-36080" yWindow="-3880" windowWidth="30600" windowHeight="18120" xr2:uid="{E4B1E5C7-DAD6-3D4D-9E2A-0CE9718F5B2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -599,7 +599,7 @@
   <dimension ref="A2:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Refactored this test, due to code refactoring- passes
Refactored tests due to code change. 3 tests for the rules_engine.rb were refactored due to code refactoring, they still test the same results and now pass again.
</commit_message>
<xml_diff>
--- a/man_tests_T1A2.xlsx
+++ b/man_tests_T1A2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shelbyd/CODING/Projects/Ruby/CA_Terminal_App_RPSLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8470F2-7517-3349-9117-424DD0F64F7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A128A759-8D3D-DB4E-9462-DF05A4320A5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36080" yWindow="-3880" windowWidth="30600" windowHeight="18120" xr2:uid="{E4B1E5C7-DAD6-3D4D-9E2A-0CE9718F5B2E}"/>
+    <workbookView xWindow="0" yWindow="2860" windowWidth="30600" windowHeight="16280" xr2:uid="{E4B1E5C7-DAD6-3D4D-9E2A-0CE9718F5B2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Feature being tested</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Out come will be 1 as 1 point was added</t>
+  </si>
+  <si>
+    <t>made famous by the Big Bang Theory, this is ROCK PAPER SCISSORS SPOCK LIZARD!</t>
   </si>
 </sst>
 </file>
@@ -596,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB52CDC-51B2-5744-8C62-74681603DE00}">
-  <dimension ref="A2:I24"/>
+  <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1070,6 +1073,11 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
     </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>